<commit_message>
fixed naming of post test column
</commit_message>
<xml_diff>
--- a/postTestConditions.xlsx
+++ b/postTestConditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasY21\Dropbox\Documents\Prep\Koehnlein\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3281DE2-1177-4C68-8E1C-3340059E110D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DCAD35-16B7-459D-BB53-D7751E14FC23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6795" yWindow="3405" windowWidth="14400" windowHeight="8415" xr2:uid="{21124619-A3FC-413F-B9E6-3C5CB39C34F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{21124619-A3FC-413F-B9E6-3C5CB39C34F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>postTest/86_totipa1.wav</t>
   </si>
   <si>
-    <t>audioC</t>
+    <t>audioX</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>

</xml_diff>